<commit_message>
Add All Remaining pages/Tests till requirement
</commit_message>
<xml_diff>
--- a/src/test/java/Address/Address.xlsx
+++ b/src/test/java/Address/Address.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Foodics\AmazonTask\Foodics_Amazon_Task\src\test\java\Address\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8F0D5A-997C-4429-8EC2-5A7A9A17865E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364946E8-8A7D-43DA-8682-F2A1D45F6C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -403,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,10 +480,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>